<commit_message>
Add victim age and offense category/groupings for demos
</commit_message>
<xml_diff>
--- a/nibrs/r-load/NIBRSCodeTables.xlsx
+++ b/nibrs/r-load/NIBRSCodeTables.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="11595" windowHeight="8190" tabRatio="705" firstSheet="16" activeTab="20"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="11595" windowHeight="8190" tabRatio="705" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="TOC" sheetId="1" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="880" uniqueCount="688">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="938" uniqueCount="691">
   <si>
     <t>Table</t>
   </si>
@@ -2106,6 +2106,15 @@
   </si>
   <si>
     <t>Juvenile/No Custody</t>
+  </si>
+  <si>
+    <t>OffenseCategory1</t>
+  </si>
+  <si>
+    <t>Simple Assault</t>
+  </si>
+  <si>
+    <t>Serious Violence</t>
   </si>
 </sst>
 </file>
@@ -5104,7 +5113,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
@@ -6417,10 +6426,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C58"/>
+  <dimension ref="A1:D58"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A59" sqref="A59"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E45" sqref="E45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -6428,10 +6437,11 @@
     <col min="1" max="1" width="20.875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="19.375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="57.125" bestFit="1" customWidth="1"/>
-    <col min="4" max="1025" width="10.625"/>
+    <col min="4" max="4" width="16.75" customWidth="1"/>
+    <col min="5" max="1025" width="10.625"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>525</v>
       </c>
@@ -6441,8 +6451,11 @@
       <c r="C1" t="s">
         <v>526</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D1" t="s">
+        <v>688</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>91</v>
       </c>
@@ -6452,8 +6465,11 @@
       <c r="C2" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D2" t="s">
+        <v>690</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>92</v>
       </c>
@@ -6463,8 +6479,11 @@
       <c r="C3" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D3" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>93</v>
       </c>
@@ -6474,8 +6493,11 @@
       <c r="C4" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D4" s="1" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>100</v>
       </c>
@@ -6485,8 +6507,11 @@
       <c r="C5" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D5" s="1" t="s">
+        <v>690</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>120</v>
       </c>
@@ -6496,8 +6521,11 @@
       <c r="C6" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D6" s="1" t="s">
+        <v>690</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>131</v>
       </c>
@@ -6507,8 +6535,11 @@
       <c r="C7" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D7" s="1" t="s">
+        <v>690</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>132</v>
       </c>
@@ -6518,8 +6549,11 @@
       <c r="C8" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D8" t="s">
+        <v>689</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>133</v>
       </c>
@@ -6529,8 +6563,11 @@
       <c r="C9" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="10" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D9" s="1" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>200</v>
       </c>
@@ -6540,8 +6577,11 @@
       <c r="C10" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="11" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D10" s="1" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>210</v>
       </c>
@@ -6551,8 +6591,11 @@
       <c r="C11" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="12" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D11" s="1" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>220</v>
       </c>
@@ -6562,8 +6605,11 @@
       <c r="C12" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="13" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D12" s="1" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>231</v>
       </c>
@@ -6573,8 +6619,11 @@
       <c r="C13" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="14" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D13" s="1" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>232</v>
       </c>
@@ -6584,8 +6633,11 @@
       <c r="C14" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="15" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D14" s="1" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>233</v>
       </c>
@@ -6595,8 +6647,11 @@
       <c r="C15" t="s">
         <v>71</v>
       </c>
-    </row>
-    <row r="16" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D15" s="1" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>234</v>
       </c>
@@ -6606,8 +6661,11 @@
       <c r="C16" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="17" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D16" s="1" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>235</v>
       </c>
@@ -6617,8 +6675,11 @@
       <c r="C17" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="18" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D17" s="1" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>236</v>
       </c>
@@ -6628,8 +6689,11 @@
       <c r="C18" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="19" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D18" s="1" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>237</v>
       </c>
@@ -6639,8 +6703,11 @@
       <c r="C19" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="20" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D19" s="1" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>238</v>
       </c>
@@ -6650,8 +6717,11 @@
       <c r="C20" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="21" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D20" s="1" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>240</v>
       </c>
@@ -6661,8 +6731,11 @@
       <c r="C21" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="22" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D21" s="1" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>250</v>
       </c>
@@ -6672,8 +6745,11 @@
       <c r="C22" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="23" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D22" s="1" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>261</v>
       </c>
@@ -6683,8 +6759,11 @@
       <c r="C23" t="s">
         <v>85</v>
       </c>
-    </row>
-    <row r="24" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D23" s="1" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>262</v>
       </c>
@@ -6694,8 +6773,11 @@
       <c r="C24" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="25" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D24" s="1" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>263</v>
       </c>
@@ -6705,8 +6787,11 @@
       <c r="C25" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="26" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D25" s="1" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>264</v>
       </c>
@@ -6716,8 +6801,11 @@
       <c r="C26" t="s">
         <v>91</v>
       </c>
-    </row>
-    <row r="27" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D26" s="1" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>265</v>
       </c>
@@ -6727,8 +6815,11 @@
       <c r="C27" t="s">
         <v>93</v>
       </c>
-    </row>
-    <row r="28" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D27" s="1" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>270</v>
       </c>
@@ -6738,8 +6829,11 @@
       <c r="C28" t="s">
         <v>94</v>
       </c>
-    </row>
-    <row r="29" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D28" s="1" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>290</v>
       </c>
@@ -6749,8 +6843,11 @@
       <c r="C29" t="s">
         <v>95</v>
       </c>
-    </row>
-    <row r="30" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D29" s="1" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>351</v>
       </c>
@@ -6760,8 +6857,11 @@
       <c r="C30" t="s">
         <v>97</v>
       </c>
-    </row>
-    <row r="31" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D30" s="1" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>352</v>
       </c>
@@ -6771,8 +6871,11 @@
       <c r="C31" t="s">
         <v>99</v>
       </c>
-    </row>
-    <row r="32" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D31" s="1" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>370</v>
       </c>
@@ -6782,8 +6885,11 @@
       <c r="C32" t="s">
         <v>100</v>
       </c>
-    </row>
-    <row r="33" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D32" s="1" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>391</v>
       </c>
@@ -6793,8 +6899,11 @@
       <c r="C33" t="s">
         <v>102</v>
       </c>
-    </row>
-    <row r="34" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D33" s="1" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>392</v>
       </c>
@@ -6804,8 +6913,11 @@
       <c r="C34" t="s">
         <v>104</v>
       </c>
-    </row>
-    <row r="35" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D34" s="1" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>393</v>
       </c>
@@ -6815,8 +6927,11 @@
       <c r="C35" t="s">
         <v>106</v>
       </c>
-    </row>
-    <row r="36" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D35" s="1" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>394</v>
       </c>
@@ -6826,8 +6941,11 @@
       <c r="C36" t="s">
         <v>108</v>
       </c>
-    </row>
-    <row r="37" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D36" s="1" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>401</v>
       </c>
@@ -6837,8 +6955,11 @@
       <c r="C37" t="s">
         <v>110</v>
       </c>
-    </row>
-    <row r="38" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D37" s="1" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>402</v>
       </c>
@@ -6848,8 +6969,11 @@
       <c r="C38" t="s">
         <v>112</v>
       </c>
-    </row>
-    <row r="39" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D38" s="1" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>510</v>
       </c>
@@ -6859,8 +6983,11 @@
       <c r="C39" t="s">
         <v>113</v>
       </c>
-    </row>
-    <row r="40" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D39" s="1" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>111</v>
       </c>
@@ -6870,8 +6997,11 @@
       <c r="C40" t="s">
         <v>115</v>
       </c>
-    </row>
-    <row r="41" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D40" s="1" t="s">
+        <v>690</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>112</v>
       </c>
@@ -6881,8 +7011,11 @@
       <c r="C41" t="s">
         <v>117</v>
       </c>
-    </row>
-    <row r="42" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D41" s="1" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>113</v>
       </c>
@@ -6892,8 +7025,11 @@
       <c r="C42" t="s">
         <v>119</v>
       </c>
-    </row>
-    <row r="43" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D42" s="1" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>114</v>
       </c>
@@ -6903,8 +7039,11 @@
       <c r="C43" t="s">
         <v>121</v>
       </c>
-    </row>
-    <row r="44" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D43" s="1" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>280</v>
       </c>
@@ -6914,8 +7053,11 @@
       <c r="C44" t="s">
         <v>122</v>
       </c>
-    </row>
-    <row r="45" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D44" s="1" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>361</v>
       </c>
@@ -6925,8 +7067,11 @@
       <c r="C45" t="s">
         <v>124</v>
       </c>
-    </row>
-    <row r="46" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D45" s="1" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>362</v>
       </c>
@@ -6936,8 +7081,11 @@
       <c r="C46" t="s">
         <v>126</v>
       </c>
-    </row>
-    <row r="47" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D46" s="1" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>520</v>
       </c>
@@ -6947,8 +7095,11 @@
       <c r="C47" t="s">
         <v>127</v>
       </c>
-    </row>
-    <row r="48" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D47" s="1" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>901</v>
       </c>
@@ -6958,8 +7109,11 @@
       <c r="C48" t="s">
         <v>129</v>
       </c>
-    </row>
-    <row r="49" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D48" s="1" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>902</v>
       </c>
@@ -6969,8 +7123,11 @@
       <c r="C49" t="s">
         <v>131</v>
       </c>
-    </row>
-    <row r="50" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D49" s="1" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>903</v>
       </c>
@@ -6980,8 +7137,11 @@
       <c r="C50" t="s">
         <v>133</v>
       </c>
-    </row>
-    <row r="51" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D50" s="1" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>904</v>
       </c>
@@ -6991,8 +7151,11 @@
       <c r="C51" t="s">
         <v>135</v>
       </c>
-    </row>
-    <row r="52" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D51" s="1" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A52">
         <v>905</v>
       </c>
@@ -7002,8 +7165,11 @@
       <c r="C52" t="s">
         <v>137</v>
       </c>
-    </row>
-    <row r="53" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D52" s="1" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A53">
         <v>906</v>
       </c>
@@ -7013,8 +7179,11 @@
       <c r="C53" t="s">
         <v>139</v>
       </c>
-    </row>
-    <row r="54" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D53" s="1" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A54">
         <v>907</v>
       </c>
@@ -7024,8 +7193,11 @@
       <c r="C54" t="s">
         <v>141</v>
       </c>
-    </row>
-    <row r="55" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D54" s="1" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A55">
         <v>908</v>
       </c>
@@ -7035,8 +7207,11 @@
       <c r="C55" t="s">
         <v>143</v>
       </c>
-    </row>
-    <row r="56" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D55" s="1" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A56">
         <v>909</v>
       </c>
@@ -7046,8 +7221,11 @@
       <c r="C56" t="s">
         <v>145</v>
       </c>
-    </row>
-    <row r="57" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D56" s="1" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A57">
         <v>910</v>
       </c>
@@ -7057,8 +7235,11 @@
       <c r="C57" t="s">
         <v>147</v>
       </c>
-    </row>
-    <row r="58" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D57" s="1" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A58">
         <v>990</v>
       </c>
@@ -7067,6 +7248,9 @@
       </c>
       <c r="C58" t="s">
         <v>149</v>
+      </c>
+      <c r="D58" s="1" t="s">
+        <v>277</v>
       </c>
     </row>
   </sheetData>

</xml_diff>